<commit_message>
test cases name added
</commit_message>
<xml_diff>
--- a/testCases-Dilruba/Test _cases_costco.xlsx
+++ b/testCases-Dilruba/Test _cases_costco.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14038\Documents\piit\Homeworks\homework5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E7B45-4E9F-47CE-9DA8-BE9A818160DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0183BD-BB57-4A74-BFF2-5C0B24067D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="walmart_test_cases" sheetId="2" r:id="rId2"/>
+    <sheet name="costco_test_cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1257,7 +1257,7 @@
   <dimension ref="A1:I641"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>